<commit_message>
fix: README, TestCase (for Noveo)
</commit_message>
<xml_diff>
--- a/TestDocumentation/TestCase (for Noveo).xlsx
+++ b/TestDocumentation/TestCase (for Noveo).xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_Slack\TestDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3AD220-77A0-45A0-B9E2-C2F9E3C4049D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829D4703-AA84-4E83-9834-AFA0569153B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskDescription" sheetId="6" r:id="rId1"/>
     <sheet name="TestCases" sheetId="1" r:id="rId2"/>
     <sheet name="BugReport" sheetId="5" r:id="rId3"/>
-    <sheet name="Requirements" sheetId="4" r:id="rId4"/>
+    <sheet name="Recommendations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1344,9 +1344,6 @@
     <t>2. Change the http protocol to https, because this is a registration form and it contains personal data.</t>
   </si>
   <si>
-    <t>Requirements</t>
-  </si>
-  <si>
     <t>https://github.com/Baray44/QA_Slack/blob/master/TestDocumentation/BugReport/Bug%20(noveogroup.com)/BG-01.png</t>
   </si>
   <si>
@@ -1405,6 +1402,9 @@
   </si>
   <si>
     <t>https://github.com/Baray44/QA_Slack/blob/master/TestDocumentation/BugReport/Bug%20(noveogroup.com)/BG-20.png</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
   </si>
 </sst>
 </file>
@@ -2362,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A52B761-0B4F-4757-B889-8C6A519D35A0}">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -4430,7 +4430,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="55" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4462,7 +4462,7 @@
         <v>24</v>
       </c>
       <c r="J3" s="55" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -4494,7 +4494,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4526,7 +4526,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4558,7 +4558,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4590,7 +4590,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
         <v>24</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4654,7 +4654,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4686,7 +4686,7 @@
         <v>24</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="142.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -4718,7 +4718,7 @@
         <v>24</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4750,7 +4750,7 @@
         <v>24</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.3">
@@ -4782,7 +4782,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4814,7 +4814,7 @@
         <v>24</v>
       </c>
       <c r="J14" s="55" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4846,7 +4846,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4878,7 +4878,7 @@
         <v>24</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4910,7 +4910,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="55" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -4942,7 +4942,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="55" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
@@ -4974,7 +4974,7 @@
         <v>24</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5006,7 +5006,7 @@
         <v>347</v>
       </c>
       <c r="J20" s="55" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5038,7 +5038,7 @@
         <v>353</v>
       </c>
       <c r="J21" s="55" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -5072,8 +5072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3812933C-CF38-4F37-9768-0BF7A411BAA2}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5083,7 +5083,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>